<commit_message>
Correcciones de version 1
</commit_message>
<xml_diff>
--- a/BACKEND/uploads/archivo_subido.xlsx
+++ b/BACKEND/uploads/archivo_subido.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sena\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F59068-E41F-4035-B44B-161013D6B8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05ABD33-4005-4A49-A7CA-7C7022D02329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="4965" windowWidth="14040" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>TIPO DE DOCUMENTO</t>
   </si>
@@ -49,16 +49,28 @@
     <t>MAYO</t>
   </si>
   <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>ejemplo tipo</t>
+  </si>
+  <si>
     <t>JUNIO</t>
   </si>
   <si>
+    <t>YAIR MAL</t>
+  </si>
+  <si>
+    <t>FALLECIDO</t>
+  </si>
+  <si>
     <t>FEBRERO</t>
   </si>
   <si>
-    <t>FALLECIDO</t>
-  </si>
-  <si>
-    <t>YAIR MAL</t>
+    <t>PPT</t>
+  </si>
+  <si>
+    <t>MARZO</t>
   </si>
   <si>
     <t>JOSE URBANO PARRA GUZMAN</t>
@@ -67,23 +79,23 @@
     <t>SEPTIEMBRE</t>
   </si>
   <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>OCTUBRE</t>
+  </si>
+  <si>
     <t>ANTONIO  CASTAÑEDA</t>
   </si>
   <si>
-    <t>MARZO</t>
-  </si>
-  <si>
     <t>ARNULFO  BRIÑEZ QUESADA</t>
-  </si>
-  <si>
-    <t>OCTUBRE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,12 +107,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,12 +144,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -447,16 +452,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="3" width="29" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
     <col min="4" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -502,19 +508,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>1108453116</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F3">
         <v>2024</v>
@@ -525,83 +531,158 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>21202856</v>
+        <v>1108453116</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
       <c r="F4">
-        <v>1985</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
-        <v>5814634</v>
+      <c r="B5">
+        <v>21202856</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5">
-        <v>1962</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5817677</v>
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>1108453116</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
       </c>
       <c r="F6">
-        <v>1964</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>5999992</v>
+      <c r="B7">
+        <v>5814634</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
       </c>
       <c r="F7">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>1108453116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5817677</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5999992</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10">
         <v>1971</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Entrada inválida" error="Debe seleccionar uno de los valores válidos: CC, TI, CE, PPT" promptTitle="Tipo de Documento" prompt="Seleccione un tipo de documento válido: CC, TI, CE, PPT" sqref="A2:A1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"CC,TI,CE,PPT"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Día inválido" error="El día debe ser un número entre 1 y 31" promptTitle="Día" prompt="Ingrese un día válido (1-31)" sqref="D2:D1000" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>1</formula1>
+      <formula2>31</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Mes inválido" error="Debe seleccionar un mes válido en mayúsculas" promptTitle="Mes" prompt="Seleccione un mes válido" sqref="E2:E1000" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>"ENERO,FEBRERO,MARZO,ABRIL,MAYO,JUNIO,JULIO,AGOSTO,SEPTIEMBRE,OCTUBRE,NOVIEMBRE,DICIEMBRE"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorTitle="Año inválido" error="El año debe estar entre 1900 y 2025 (no se permiten años futuros)" promptTitle="Año" prompt="Ingrese un año válido (1900-2025)" sqref="F2:F1000" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>1900</formula1>
+      <formula2>2025</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>